<commit_message>
Main functions to add new/edit old exerciseAbstract object - Dao - Repository - ViewModel
Signed-off-by: Tamir Mishali <tamirmishali@gmail.com>
</commit_message>
<xml_diff>
--- a/New_exercise_db_tables.xlsx
+++ b/New_exercise_db_tables.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Tamir\Projects\TrainingManager\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{987ECC37-10D8-481C-B1AF-6B9300CD7058}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C40A9571-BF45-4F11-AE36-C95F8BB7EECC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="1170" yWindow="1170" windowWidth="25080" windowHeight="13545" activeTab="2" xr2:uid="{8EF91394-A5DA-4302-A49F-F86034EFE3BF}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{8EF91394-A5DA-4302-A49F-F86034EFE3BF}"/>
   </bookViews>
   <sheets>
-    <sheet name="practical_ex" sheetId="6" r:id="rId1"/>
+    <sheet name="ExerciseAbstract" sheetId="6" r:id="rId1"/>
     <sheet name="Table_arrangement_1" sheetId="7" state="hidden" r:id="rId2"/>
     <sheet name="Table_arrangement_2" sheetId="8" r:id="rId3"/>
     <sheet name="General_Tables" sheetId="9" r:id="rId4"/>
@@ -6468,7 +6468,7 @@
   <dimension ref="A1:Q41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
major fix in add_edit_exerviseAbstract - db reload from a built one - added DAO's without viewmodel
Signed-off-by: Tamir Mishali <tamirmishali@gmail.com>
</commit_message>
<xml_diff>
--- a/New_exercise_db_tables.xlsx
+++ b/New_exercise_db_tables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Tamir\Projects\TrainingManager\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C40A9571-BF45-4F11-AE36-C95F8BB7EECC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67C6E038-A3A0-466A-A3AE-D083342ACD05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{8EF91394-A5DA-4302-A49F-F86034EFE3BF}"/>
   </bookViews>
@@ -1091,13 +1091,13 @@
       <xdr:col>12</xdr:col>
       <xdr:colOff>47625</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:rowOff>123824</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>1228725</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>38099</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1112,8 +1112,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="12134850" y="2800350"/>
-          <a:ext cx="1790700" cy="1181100"/>
+          <a:off x="12011025" y="2800349"/>
+          <a:ext cx="1790700" cy="4486275"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1913,7 +1913,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>INSERT INTO exerciseabs_operation (id_exerciseabs_info_value, value)</a:t>
+            <a:t>INSERT INTO exerciseabs_operation (id_exerciseabs_info_value, operation)</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -1952,7 +1952,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>INSERT INTO exerciseabs_operation (id_exerciseabs_info_value, value)</a:t>
+            <a:t>INSERT INTO exerciseabs_operation (id_exerciseabs_info_value, operation)</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -1991,7 +1991,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>INSERT INTO exerciseabs_operation (id_exerciseabs_info_value, value)</a:t>
+            <a:t>INSERT INTO exerciseabs_operation (id_exerciseabs_info_value, operation)</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -2052,7 +2052,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>INSERT INTO exerciseabs_operation (id_exerciseabs_info_value, value)</a:t>
+            <a:t>INSERT INTO exerciseabs_operation (id_exerciseabs_info_value, operation)</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -2091,7 +2091,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>INSERT INTO exerciseabs_operation (id_exerciseabs_info_value, value)</a:t>
+            <a:t>INSERT INTO exerciseabs_operation (id_exerciseabs_info_value, operation)</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -2130,7 +2130,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>INSERT INTO exerciseabs_operation (id_exerciseabs_info_value, value)</a:t>
+            <a:t>INSERT INTO exerciseabs_operation (id_exerciseabs_info_value, operation)</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -2169,7 +2169,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>INSERT INTO exerciseabs_operation (id_exerciseabs_info_value, value)</a:t>
+            <a:t>INSERT INTO exerciseabs_operation (id_exerciseabs_info_value, operation)</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -2230,7 +2230,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>INSERT INTO exerciseabs_operation (id_exerciseabs_info_value, value)</a:t>
+            <a:t>INSERT INTO exerciseabs_operation (id_exerciseabs_info_value, operation)</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -2269,7 +2269,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>INSERT INTO exerciseabs_operation (id_exerciseabs_info_value, value)</a:t>
+            <a:t>INSERT INTO exerciseabs_operation (id_exerciseabs_info_value, operation)</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -2308,7 +2308,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>INSERT INTO exerciseabs_operation (id_exerciseabs_info_value, value)</a:t>
+            <a:t>INSERT INTO exerciseabs_operation (id_exerciseabs_info_value, operation)</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -2347,7 +2347,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>INSERT INTO exerciseabs_operation (id_exerciseabs_info_value, value)</a:t>
+            <a:t>INSERT INTO exerciseabs_operation (id_exerciseabs_info_value, operation)</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -2386,7 +2386,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>INSERT INTO exerciseabs_operation (id_exerciseabs_info_value, value)</a:t>
+            <a:t>INSERT INTO exerciseabs_operation (id_exerciseabs_info_value, operation)</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -2425,7 +2425,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>INSERT INTO exerciseabs_operation (id_exerciseabs_info_value, value)</a:t>
+            <a:t>INSERT INTO exerciseabs_operation (id_exerciseabs_info_value, operation)</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -2464,7 +2464,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>INSERT INTO exerciseabs_operation (id_exerciseabs_info_value, value)</a:t>
+            <a:t>INSERT INTO exerciseabs_operation (id_exerciseabs_info_value, operation)</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -2503,7 +2503,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>INSERT INTO exerciseabs_operation (id_exerciseabs_info_value, value)</a:t>
+            <a:t>INSERT INTO exerciseabs_operation (id_exerciseabs_info_value, operation)</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -2542,7 +2542,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>INSERT INTO exerciseabs_operation (id_exerciseabs_info_value, value)</a:t>
+            <a:t>INSERT INTO exerciseabs_operation (id_exerciseabs_info_value, operation)</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -2592,7 +2592,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>INSERT INTO exerciseabs_operation (id_exerciseabs_info_value, value)</a:t>
+            <a:t>INSERT INTO exerciseabs_operation (id_exerciseabs_info_value, operation)</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -2631,7 +2631,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>INSERT INTO exerciseabs_operation (id_exerciseabs_info_value, value)</a:t>
+            <a:t>INSERT INTO exerciseabs_operation (id_exerciseabs_info_value, operation)</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -2670,7 +2670,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>INSERT INTO exerciseabs_operation (id_exerciseabs_info_value, value)</a:t>
+            <a:t>INSERT INTO exerciseabs_operation (id_exerciseabs_info_value, operation)</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -2709,7 +2709,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>INSERT INTO exerciseabs_operation (id_exerciseabs_info_value, value)</a:t>
+            <a:t>INSERT INTO exerciseabs_operation (id_exerciseabs_info_value, operation)</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -2748,7 +2748,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>INSERT INTO exerciseabs_operation (id_exerciseabs_info_value, value)</a:t>
+            <a:t>INSERT INTO exerciseabs_operation (id_exerciseabs_info_value, operation)</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -2787,7 +2787,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>INSERT INTO exerciseabs_operation (id_exerciseabs_info_value, value)</a:t>
+            <a:t>INSERT INTO exerciseabs_operation (id_exerciseabs_info_value, operation)</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -2826,7 +2826,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>INSERT INTO exerciseabs_operation (id_exerciseabs_info_value, value)</a:t>
+            <a:t>INSERT INTO exerciseabs_operation (id_exerciseabs_info_value, operation)</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -2876,7 +2876,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>INSERT INTO exerciseabs_operation (id_exerciseabs_info_value, value)</a:t>
+            <a:t>INSERT INTO exerciseabs_operation (id_exerciseabs_info_value, operation)</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -2915,7 +2915,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>INSERT INTO exerciseabs_operation (id_exerciseabs_info_value, value)</a:t>
+            <a:t>INSERT INTO exerciseabs_operation (id_exerciseabs_info_value, operation)</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -2954,7 +2954,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>INSERT INTO exerciseabs_operation (id_exerciseabs_info_value, value)</a:t>
+            <a:t>INSERT INTO exerciseabs_operation (id_exerciseabs_info_value, operation)</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -2993,7 +2993,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>INSERT INTO exerciseabs_operation (id_exerciseabs_info_value, value)</a:t>
+            <a:t>INSERT INTO exerciseabs_operation (id_exerciseabs_info_value, operation)</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -6467,8 +6467,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4C54436-ED1B-41D0-8717-BF6247E69E75}">
   <dimension ref="A1:Q41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
backup commit - poppig keyboard not going away when switching views - fixed - listener on new inserted EA and passing id back to ui acivity - small db change - int to Integer on nickname column on exerciseAbstract
Signed-off-by: Tamir Mishali <tamirmishali@gmail.com>
</commit_message>
<xml_diff>
--- a/New_exercise_db_tables.xlsx
+++ b/New_exercise_db_tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Tamir\Projects\TrainingManager\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67C6E038-A3A0-466A-A3AE-D083342ACD05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E3EDB34-9344-4F0E-9A6E-C55361ECB132}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{8EF91394-A5DA-4302-A49F-F86034EFE3BF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{8EF91394-A5DA-4302-A49F-F86034EFE3BF}"/>
   </bookViews>
   <sheets>
     <sheet name="ExerciseAbstract" sheetId="6" r:id="rId1"/>
@@ -3864,6 +3864,1387 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="13" name="TextBox 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{234A3749-0EF6-28D2-EB08-E0AD14BAD924}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="342900" y="8305800"/>
+          <a:ext cx="13973175" cy="4838700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>INSERT INTO exerciseabs_info (info_header_name)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>VALUES ('muscle');</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>INSERT INTO exerciseabs_info (info_header_name)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>VALUES ('load_type');</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>INSERT INTO exerciseabs_info (info_header_name)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>VALUES ('position');</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>INSERT INTO exerciseabs_info (info_header_name)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>VALUES ('angle');</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>INSERT INTO exerciseabs_info (info_header_name)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>VALUES ('grip_width');</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>INSERT INTO exerciseabs_info (info_header_name)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>VALUES ('thumbs_direction');</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>INSERT INTO exerciseabs_info (info_header_name)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>VALUES ('separate_hands');</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>INSERT INTO exerciseabs_info_value (id_exerciseabs_info, value)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>VALUES (1, 'Chest');</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>INSERT INTO exerciseabs_info_value (id_exerciseabs_info, value)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>VALUES (1, 'Back');</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>INSERT INTO exerciseabs_info_value (id_exerciseabs_info, value)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>VALUES (1, 'Legs');</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>INSERT INTO exerciseabs_info_value (id_exerciseabs_info, value)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>VALUES (1, 'Shoulders');</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>INSERT INTO exerciseabs_info_value (id_exerciseabs_info, value)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>VALUES (1, 'Biceps');</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>INSERT INTO exerciseabs_info_value (id_exerciseabs_info, value)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>VALUES (1, 'Triceps');</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>INSERT INTO exerciseabs_info_value (id_exerciseabs_info, value)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>VALUES (1, 'Abs');</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>INSERT INTO exerciseabs_info_value (id_exerciseabs_info, value)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>VALUES (2, 'Dumbbell');</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>INSERT INTO exerciseabs_info_value (id_exerciseabs_info, value)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>VALUES (2, 'Barbell');</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>INSERT INTO exerciseabs_info_value (id_exerciseabs_info, value)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>VALUES (2, 'Weighted belt');</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>INSERT INTO exerciseabs_info_value (id_exerciseabs_info, value)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>VALUES (2, 'Machine');</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>INSERT INTO exerciseabs_info_value (id_exerciseabs_info, value)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>VALUES (2, 'Cables');</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>INSERT INTO exerciseabs_info_value (id_exerciseabs_info, value)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>VALUES (2, 'T-bar');</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>INSERT INTO exerciseabs_info_value (id_exerciseabs_info, value)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>VALUES (2, 'W barbell');</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>INSERT INTO exerciseabs_info_value (id_exerciseabs_info, value)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>VALUES (3, '');</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>INSERT INTO exerciseabs_info_value (id_exerciseabs_info, value)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>VALUES (3, 'Bench');</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>INSERT INTO exerciseabs_info_value (id_exerciseabs_info, value)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>VALUES (3, 'Standing');</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>INSERT INTO exerciseabs_info_value (id_exerciseabs_info, value)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>VALUES (4, '');</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>INSERT INTO exerciseabs_info_value (id_exerciseabs_info, value)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>VALUES (4, '-30');</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>INSERT INTO exerciseabs_info_value (id_exerciseabs_info, value)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>VALUES (4, '-15');</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>INSERT INTO exerciseabs_info_value (id_exerciseabs_info, value)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>VALUES (4, '0');</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>INSERT INTO exerciseabs_info_value (id_exerciseabs_info, value)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>VALUES (4, '15');</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>INSERT INTO exerciseabs_info_value (id_exerciseabs_info, value)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>VALUES (4, '30');</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>INSERT INTO exerciseabs_info_value (id_exerciseabs_info, value)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>VALUES (4, '45');</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>INSERT INTO exerciseabs_info_value (id_exerciseabs_info, value)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>VALUES (4, '60');</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>INSERT INTO exerciseabs_info_value (id_exerciseabs_info, value)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>VALUES (4, '75');</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>INSERT INTO exerciseabs_info_value (id_exerciseabs_info, value)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>VALUES (4, '90');</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>INSERT INTO exerciseabs_info_value (id_exerciseabs_info, value)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>VALUES (5, '');</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>INSERT INTO exerciseabs_info_value (id_exerciseabs_info, value)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>VALUES (5, 'Wide');</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>INSERT INTO exerciseabs_info_value (id_exerciseabs_info, value)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>VALUES (5, 'Narrow');</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>INSERT INTO exerciseabs_info_value (id_exerciseabs_info, value)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>VALUES (6, '');</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>INSERT INTO exerciseabs_info_value (id_exerciseabs_info, value)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>VALUES (6, 'Up');</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>INSERT INTO exerciseabs_info_value (id_exerciseabs_info, value)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>VALUES (6, 'Inwards');</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>INSERT INTO exerciseabs_info_value (id_exerciseabs_info, value)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>VALUES (6, 'Outwards');</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>INSERT INTO exerciseabs_info_value (id_exerciseabs_info, value)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>VALUES (6, 'Top-Inwards');</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>INSERT INTO exerciseabs_info_value (id_exerciseabs_info, value)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>VALUES (7, '');</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>INSERT INTO exerciseabs_info_value (id_exerciseabs_info, value)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>VALUES (7, 'No');</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>INSERT INTO exerciseabs_info_value (id_exerciseabs_info, value)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>VALUES (7, 'Yes');</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>INSERT INTO exerciseabs_operation (id_exerciseabs_info_value, operation)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>VALUES (1, 'Pushups');</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>INSERT INTO exerciseabs_operation (id_exerciseabs_info_value, operation)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>VALUES (1, 'Press');</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>INSERT INTO exerciseabs_operation (id_exerciseabs_info_value, operation)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>VALUES (1, 'Flys');</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>INSERT INTO exerciseabs_operation (id_exerciseabs_info_value, operation)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>VALUES (2, 'Row');</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>INSERT INTO exerciseabs_operation (id_exerciseabs_info_value, operation)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>VALUES (2, 'Pullups');</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>INSERT INTO exerciseabs_operation (id_exerciseabs_info_value, operation)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>VALUES (2, 'Extension');</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>INSERT INTO exerciseabs_operation (id_exerciseabs_info_value, operation)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>VALUES (2, 'Pulldown');</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>INSERT INTO exerciseabs_operation (id_exerciseabs_info_value, operation)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>VALUES (3, 'Deadlift');</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>INSERT INTO exerciseabs_operation (id_exerciseabs_info_value, operation)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>VALUES (3, 'Squat');</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>INSERT INTO exerciseabs_operation (id_exerciseabs_info_value, operation)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>VALUES (3, 'Calf raise');</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>INSERT INTO exerciseabs_operation (id_exerciseabs_info_value, operation)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>VALUES (3, 'Hip thrust');</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>INSERT INTO exerciseabs_operation (id_exerciseabs_info_value, operation)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>VALUES (3, 'Hip adduction');</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>INSERT INTO exerciseabs_operation (id_exerciseabs_info_value, operation)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>VALUES (3, 'Hip abduction');</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>INSERT INTO exerciseabs_operation (id_exerciseabs_info_value, operation)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>VALUES (3, 'Curl');</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>INSERT INTO exerciseabs_operation (id_exerciseabs_info_value, operation)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>VALUES (3, 'Extension');</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>INSERT INTO exerciseabs_operation (id_exerciseabs_info_value, operation)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>VALUES (3, 'Pulldown');</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>INSERT INTO exerciseabs_operation (id_exerciseabs_info_value, operation)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>VALUES (4, 'Front raise');</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>INSERT INTO exerciseabs_operation (id_exerciseabs_info_value, operation)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>VALUES (4, 'Lateral raise');</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>INSERT INTO exerciseabs_operation (id_exerciseabs_info_value, operation)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>VALUES (4, 'Upright pull');</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>INSERT INTO exerciseabs_operation (id_exerciseabs_info_value, operation)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>VALUES (4, 'Face pull');</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>INSERT INTO exerciseabs_operation (id_exerciseabs_info_value, operation)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>VALUES (4, 'Delt shrag');</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>INSERT INTO exerciseabs_operation (id_exerciseabs_info_value, operation)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>VALUES (4, 'Reverse fly');</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>INSERT INTO exerciseabs_operation (id_exerciseabs_info_value, operation)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>VALUES (4, 'Press');</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>INSERT INTO exerciseabs_operation (id_exerciseabs_info_value, operation)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>VALUES (5, 'Curl');</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>INSERT INTO exerciseabs_operation (id_exerciseabs_info_value, operation)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>VALUES (6, 'Pushdown');</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>INSERT INTO exerciseabs_operation (id_exerciseabs_info_value, operation)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>VALUES (6, 'Extension');</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>INSERT INTO exerciseabs_operation (id_exerciseabs_info_value, operation)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>VALUES (6, 'Pushups');</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>INSERT INTO exerciseabs_nickname (id_exerciseabs_operation, nickname)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>VALUES (7, 'Lat');</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>INSERT INTO exerciseabs_nickname (id_exerciseabs_operation, nickname)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>VALUES (8, 'RDL');</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>INSERT INTO exerciseabs_nickname (id_exerciseabs_operation, nickname)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>VALUES (8, 'Stiff leg');</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>INSERT INTO exerciseabs_nickname (id_exerciseabs_operation, nickname)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>VALUES (8, 'Standard');</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>INSERT INTO exerciseabs_nickname (id_exerciseabs_operation, nickname)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>VALUES (9, 'Standard');</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>INSERT INTO exerciseabs_nickname (id_exerciseabs_operation, nickname)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>VALUES (9, 'Sumo');</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>INSERT INTO exerciseabs_nickname (id_exerciseabs_operation, nickname)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>VALUES (9, 'Bulgarian split');</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>INSERT INTO exerciseabs_nickname (id_exerciseabs_operation, nickname)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>VALUES (12, 'Nut crasher');</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>INSERT INTO exerciseabs_nickname (id_exerciseabs_operation, nickname)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>VALUES (13, 'not(Nut crasher)');</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>INSERT INTO exerciseabs_nickname (id_exerciseabs_operation, nickname)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>VALUES (23, 'Military');</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>INSERT INTO exerciseabs_nickname (id_exerciseabs_operation, nickname)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>VALUES (24, 'Hammer');</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>INSERT INTO exerciseabs_nickname (id_exerciseabs_operation, nickname)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>VALUES (24, 'Preacher');</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>INSERT INTO exerciseabs_nickname (id_exerciseabs_operation, nickname)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>VALUES (24, '21s');</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>INSERT INTO exerciseabs_nickname (id_exerciseabs_operation, nickname)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>VALUES (24, 'Incline waiters');</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>INSERT INTO exerciseabs_nickname (id_exerciseabs_operation, nickname)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>VALUES (27, 'Diamond');</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-IL" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -6467,8 +7848,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4C54436-ED1B-41D0-8717-BF6247E69E75}">
   <dimension ref="A1:Q41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" topLeftCell="A35" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="R49" sqref="R49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
new/edit ExcerciseAbstract logic (has errors) - Retrieved ExerciseAbstract from db using an ExerciseAbstract object
Signed-off-by: Tamir Mishali <tamirmishali@gmail.com>
</commit_message>
<xml_diff>
--- a/New_exercise_db_tables.xlsx
+++ b/New_exercise_db_tables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Tamir\Projects\TrainingManager\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E3EDB34-9344-4F0E-9A6E-C55361ECB132}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13757384-891C-4363-9F99-DED8FA38AC8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{8EF91394-A5DA-4302-A49F-F86034EFE3BF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8EF91394-A5DA-4302-A49F-F86034EFE3BF}"/>
   </bookViews>
   <sheets>
     <sheet name="ExerciseAbstract" sheetId="6" r:id="rId1"/>
@@ -789,8 +789,8 @@
     <xdr:to>
       <xdr:col>17</xdr:col>
       <xdr:colOff>581025</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -805,8 +805,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9829800" y="47625"/>
-          <a:ext cx="4791075" cy="4676775"/>
+          <a:off x="10391775" y="47625"/>
+          <a:ext cx="5162550" cy="3000375"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -916,6 +916,142 @@
           <a:r>
             <a:rPr lang="en-US" sz="1100" baseline="0"/>
             <a:t>one will construct </a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="TextBox 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6ADA5C85-70C0-BC6F-B701-3EF913CE6792}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10391775" y="3086100"/>
+          <a:ext cx="7058025" cy="2705100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>SELECT exerciseabs_table.id_exerciseabs, eaiv1.value as muscle, exerciseabs_operation.operation ,exerciseabs_nickname.nickname, </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>eaiv2.value as load_type, eaiv3.value as position, eaiv4.value as angle ,eaiv5.value as grip_width ,eaiv6.value as thumbs_direction ,eaiv7.value as separate_sides </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>FROM exerciseabs_table </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>	LEFT JOIN exerciseabs_info_value eaiv1 ON eaiv1.id = exerciseabs_table.id_muscle </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>	JOIN exerciseabs_operation ON exerciseabs_operation.id = exerciseabs_table.id_operation </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>	LEFT JOIN exerciseabs_nickname ON exerciseabs_nickname.id = exerciseabs_table.id_nickname </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>	LEFT JOIN exerciseabs_info_value eaiv2 ON eaiv2.id = exerciseabs_table.id_load_type </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>	LEFT JOIN exerciseabs_info_value eaiv3 ON eaiv3.id = exerciseabs_table.id_position </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>	LEFT JOIN exerciseabs_info_value eaiv4 ON eaiv4.id = exerciseabs_table.id_angle </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>	LEFT JOIN exerciseabs_info_value eaiv5 ON eaiv5.id = exerciseabs_table.id_grip_width </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>	LEFT JOIN exerciseabs_info_value eaiv6 ON eaiv6.id = exerciseabs_table.id_thumbs_direction </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>	LEFT JOIN exerciseabs_info_value eaiv7 ON eaiv7.id = exerciseabs_table.id_separate_sides </a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -6316,7 +6452,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -6326,8 +6462,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6315DD8-911B-453E-B313-C2DFA2753D70}">
   <dimension ref="A1:J38"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J33" sqref="J33"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O42" sqref="O42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7848,8 +7984,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4C54436-ED1B-41D0-8717-BF6247E69E75}">
   <dimension ref="A1:Q41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R49" sqref="R49"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
testAPK, Adaptation and minor bug fix - Java level 11 from 8 - Colors and fonts - many ToDo's completed and code arrangments - AnroidManifest testAPK! - EA.strip() - name changes
Signed-off-by: Tamir Mishali <tamirmishali@gmail.com>
</commit_message>
<xml_diff>
--- a/New_exercise_db_tables.xlsx
+++ b/New_exercise_db_tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Tamir\Projects\TrainingManager\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13757384-891C-4363-9F99-DED8FA38AC8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D201146-E4CF-4A30-8A86-9F6C6982B798}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8EF91394-A5DA-4302-A49F-F86034EFE3BF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{8EF91394-A5DA-4302-A49F-F86034EFE3BF}"/>
   </bookViews>
   <sheets>
     <sheet name="ExerciseAbstract" sheetId="6" r:id="rId1"/>
@@ -4382,15 +4382,6 @@
           </a:r>
         </a:p>
         <a:p>
-          <a:endParaRPr lang="en-US" sz="1100"/>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-US" sz="1100"/>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-US" sz="1100"/>
-        </a:p>
-        <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1100"/>
             <a:t>INSERT INTO exerciseabs_info_value (id_exerciseabs_info, value)</a:t>
@@ -4399,6 +4390,27 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1100"/>
+            <a:t>VALUES (2, 'Preacher bench');</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>INSERT INTO exerciseabs_info_value (id_exerciseabs_info, value)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
             <a:t>VALUES (3, '');</a:t>
           </a:r>
         </a:p>
@@ -4425,6 +4437,43 @@
             <a:rPr lang="en-US" sz="1100"/>
             <a:t>VALUES (3, 'Standing');</a:t>
           </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>INSERT INTO exerciseabs_info_value (id_exerciseabs_info, value)</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-IL">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>VALUES (3, 'Seated');</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-IL">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
         </a:p>
         <a:p>
           <a:endParaRPr lang="en-US" sz="1100"/>
@@ -6462,7 +6511,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6315DD8-911B-453E-B313-C2DFA2753D70}">
   <dimension ref="A1:J38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="O42" sqref="O42"/>
     </sheetView>
   </sheetViews>
@@ -7984,7 +8033,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4C54436-ED1B-41D0-8717-BF6247E69E75}">
   <dimension ref="A1:Q41"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A81" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added completedExercise 'v' to expandableListView - fixed getUnfilledSetsFromWorkout query
Signed-off-by: Tamir Mishali <tamirmishali@gmail.com>
</commit_message>
<xml_diff>
--- a/New_exercise_db_tables.xlsx
+++ b/New_exercise_db_tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Tamir\Projects\TrainingManager\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D201146-E4CF-4A30-8A86-9F6C6982B798}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BAA7769-D7EA-4148-99F8-FD1D2A9CAA71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{8EF91394-A5DA-4302-A49F-F86034EFE3BF}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{8EF91394-A5DA-4302-A49F-F86034EFE3BF}"/>
   </bookViews>
   <sheets>
     <sheet name="ExerciseAbstract" sheetId="6" r:id="rId1"/>
@@ -4716,6 +4716,169 @@
           </a:r>
         </a:p>
         <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>INSERT INTO </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US"/>
+            <a:t>exerciseabs_info_value (id_exerciseabs_info</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>, </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US"/>
+            <a:t>value)</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="en-US"/>
+          </a:br>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>VALUES </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US"/>
+            <a:t>(</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>6, 'Forwards'</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US"/>
+            <a:t>)</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>;</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>INSERT INTO </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US"/>
+            <a:t>exerciseabs_info_value (id_exerciseabs_info</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>, </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US"/>
+            <a:t>value)</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="en-US"/>
+          </a:br>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>VALUES </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US"/>
+            <a:t>(</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>6, 'Backwards'</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US"/>
+            <a:t>)</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>;</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
           <a:endParaRPr lang="en-US" sz="1100"/>
         </a:p>
         <a:p>
@@ -8033,8 +8196,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4C54436-ED1B-41D0-8717-BF6247E69E75}">
   <dimension ref="A1:Q41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A81" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" topLeftCell="A90" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A113" sqref="A113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>